<commit_message>
Move slurm files into separate folder
</commit_message>
<xml_diff>
--- a/conditions_files.xlsx
+++ b/conditions_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliabertoldo/My Drive (giuliabertoldo94@gmail.com)/work/github/thesis_ms_statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5002E43-C898-1F44-BC8E-B0F25ABAAEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109E098-0415-D648-BF77-A2FF106A2894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="19040" activeTab="2" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19040" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
   </bookViews>
   <sheets>
     <sheet name="timings" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="125">
   <si>
     <t>test_pb_no_orb_no_k_15.csv</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Runs 10 meta + error + performance</t>
-  </si>
-  <si>
     <t>test_pb_mod_orb_mod_k_15.csv</t>
   </si>
   <si>
@@ -344,6 +341,78 @@
   </si>
   <si>
     <t>PB STR - ORB MOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 sim </t>
+  </si>
+  <si>
+    <t>test_pb_no_orb_str_k_15.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_no_orb_no_k_30.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_no_orb_no_k_70.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_no_orb_str_k_30.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_no_orb_str_k_70.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_no_k_15.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_no_k_30.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_no_k_70.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_str_k_15.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_str_k_30.slurm</t>
+  </si>
+  <si>
+    <t>test_pb_str_orb_str_k_70.slurm</t>
+  </si>
+  <si>
+    <t>30:59</t>
+  </si>
+  <si>
+    <t>13:27</t>
+  </si>
+  <si>
+    <t>7:02</t>
+  </si>
+  <si>
+    <t>6:45</t>
+  </si>
+  <si>
+    <t>7:57</t>
+  </si>
+  <si>
+    <t>5:17</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>4:40</t>
+  </si>
+  <si>
+    <t>5:47</t>
+  </si>
+  <si>
+    <t>8:34</t>
+  </si>
+  <si>
+    <t>8:36</t>
+  </si>
+  <si>
+    <t>10:23</t>
   </si>
 </sst>
 </file>
@@ -394,10 +463,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,52 +785,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC89430C-4702-7343-A775-7A4C1EF97FAB}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
+        <v>73</v>
+      </c>
+      <c r="E3">
+        <v>60159774</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -767,7 +844,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4">
+        <v>60161651</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -775,7 +861,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5">
+        <v>60161679</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -783,80 +878,161 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>76</v>
       </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7">
+        <v>60161585</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8">
+        <v>60161708</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9">
+        <v>60161882</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11">
+        <v>60161739</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12">
+        <v>60161749</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13">
+        <v>60161885</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15">
+        <v>60161788</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16">
+        <v>60161799</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>86</v>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17">
+        <v>60161887</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -882,25 +1058,25 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -921,7 +1097,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -939,7 +1115,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -957,7 +1133,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -975,92 +1151,92 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s">
         <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1072,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6071F97B-800A-114B-8C38-F1E7DA48221D}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,30 +1286,27 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -1152,30 +1325,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="s">
-        <v>36</v>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -1187,303 +1357,240 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="F20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="F21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
-      <c r="F27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>15</v>
       </c>
-      <c r="F28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="F29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
       </c>
-      <c r="F35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>18</v>
       </c>
-      <c r="F36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>19</v>
       </c>
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F43" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>39</v>
-      </c>
-      <c r="F45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>49</v>
       </c>
-      <c r="F51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>51</v>
       </c>
-      <c r="F53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
         <v>55</v>
       </c>
-      <c r="B59" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>56</v>
       </c>
-      <c r="F59" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F60" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>58</v>
       </c>
-      <c r="F61" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
         <v>62</v>
       </c>
-      <c r="B67" t="s">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="F67" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F68" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="1" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
         <v>65</v>
       </c>
-      <c r="F69" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move slurm scripts in folder
</commit_message>
<xml_diff>
--- a/conditions_files.xlsx
+++ b/conditions_files.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliabertoldo/My Drive (giuliabertoldo94@gmail.com)/work/github/thesis_ms_statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109E098-0415-D648-BF77-A2FF106A2894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB91376-837F-5046-83B5-566F65A198AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19040" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
   </bookViews>
   <sheets>
-    <sheet name="timings" sheetId="3" r:id="rId1"/>
-    <sheet name="final" sheetId="4" r:id="rId2"/>
+    <sheet name="final" sheetId="4" r:id="rId1"/>
+    <sheet name="timings" sheetId="3" r:id="rId2"/>
     <sheet name="overview" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="208">
   <si>
     <t>test_pb_no_orb_no_k_15.csv</t>
   </si>
@@ -325,12 +325,6 @@
     <t>pb_no_orb_mod_k_15.csv</t>
   </si>
   <si>
-    <t>pb_no_mod_mod_k_30.csv</t>
-  </si>
-  <si>
-    <t>pb_no_mod_mod_k_70.csv</t>
-  </si>
-  <si>
     <t>PB MOD - ORB MOD</t>
   </si>
   <si>
@@ -413,6 +407,261 @@
   </si>
   <si>
     <t>10:23</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_no_k_15.R</t>
+  </si>
+  <si>
+    <t>pb_no_orb_no_k_15.slurm</t>
+  </si>
+  <si>
+    <t>pb_no_orb_no_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_no_k_70.R</t>
+  </si>
+  <si>
+    <t>pb_no_orb_no_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_no_k_30.R</t>
+  </si>
+  <si>
+    <t>55012880_*</t>
+  </si>
+  <si>
+    <t>55013053_*</t>
+  </si>
+  <si>
+    <t>55013161_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_str_k_15.slurm</t>
+  </si>
+  <si>
+    <t>55013275_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_str_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_str_k_15.R</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_str_k_30.R</t>
+  </si>
+  <si>
+    <t>55013383_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_str_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_str_k_70.R</t>
+  </si>
+  <si>
+    <t>55013491_*</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_mod_k_15.R</t>
+  </si>
+  <si>
+    <t>pb_no_orb_mod_k_15.slurm</t>
+  </si>
+  <si>
+    <t>55013602_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_mod_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_mod_k_30.R</t>
+  </si>
+  <si>
+    <t>55013712_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_mod_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_no_orb_mod_k_70.R</t>
+  </si>
+  <si>
+    <t>55013835_*</t>
+  </si>
+  <si>
+    <t>pb_no_orb_mod_mod_k_30.csv</t>
+  </si>
+  <si>
+    <t>pb_no_orb_mod_mod_k_70.csv</t>
+  </si>
+  <si>
+    <t>pb_str_orb_no_k_15.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_no_k_15.R</t>
+  </si>
+  <si>
+    <t>55013945_*</t>
+  </si>
+  <si>
+    <t>pb_str_orb_no_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_no_k_30.R</t>
+  </si>
+  <si>
+    <t>55014055_*</t>
+  </si>
+  <si>
+    <t>pb_str_orb_no_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_no_k_70.R</t>
+  </si>
+  <si>
+    <t>55014171_*</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_no_k_15.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_no_k_15.R</t>
+  </si>
+  <si>
+    <t>55014411_*</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_no_k_30.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_no_k_30.slurm</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_no_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_no_k_70.R</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>55014534_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55014642_* </t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_str_k_70.R</t>
+  </si>
+  <si>
+    <t>pb_str_orb_str_k_15.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_str_k_15.R</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_str_k_30.R</t>
+  </si>
+  <si>
+    <t>pb_str_orb_str_k_30.slurm</t>
+  </si>
+  <si>
+    <t>pb_str_orb_str_k_70.slurm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55014750_* </t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_mod_k_15.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_mod_k_15.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_mod_k_30.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_mod_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_mod_k_70.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_mod_k_70.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_str_k_15.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_str_k_15.slurm</t>
+  </si>
+  <si>
+    <t>55014869_*</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_str_k_30.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_str_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_mod_orb_str_k_70.R</t>
+  </si>
+  <si>
+    <t>pb_mod_orb_str_k_70.slurm</t>
+  </si>
+  <si>
+    <t>55015088_*</t>
+  </si>
+  <si>
+    <t>55015197_*</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_mod_k_15.R</t>
+  </si>
+  <si>
+    <t>pb_str_orb_mod_k_15.slurm</t>
+  </si>
+  <si>
+    <t>pb_str_orb_mod_k_30.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_mod_k_30.R</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_mod_k_70.R</t>
+  </si>
+  <si>
+    <t>pb_str_orb_mod_k_70.slurm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55015306_* </t>
+  </si>
+  <si>
+    <t>55015416_*</t>
+  </si>
+  <si>
+    <t>55015525_*</t>
+  </si>
+  <si>
+    <t>55015635_*</t>
+  </si>
+  <si>
+    <t>55015924_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55016033_* </t>
+  </si>
+  <si>
+    <t>55016144_*</t>
+  </si>
+  <si>
+    <t>55016271_*</t>
   </si>
 </sst>
 </file>
@@ -463,12 +712,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,11 +1034,625 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666AD224-D931-1143-89FE-A13359F405FC}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="6">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="6">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="6">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="6">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="6">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="6">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="6">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="6">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="6">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="6">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" s="6">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="6">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="6">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="7">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="6">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="6">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" t="s">
+        <v>176</v>
+      </c>
+      <c r="E24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" s="6">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" t="s">
+        <v>203</v>
+      </c>
+      <c r="F25" s="6">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>169</v>
+      </c>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="6">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" t="s">
+        <v>193</v>
+      </c>
+      <c r="F28" s="6">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E29" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="6">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="6">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>188</v>
+      </c>
+      <c r="D32" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="6">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" s="6">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" t="s">
+        <v>204</v>
+      </c>
+      <c r="F35" s="6">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" t="s">
+        <v>205</v>
+      </c>
+      <c r="F36" s="6">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="6">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC89430C-4702-7343-A775-7A4C1EF97FAB}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +1702,7 @@
         <v>60159774</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -847,13 +1713,13 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4">
         <v>60161651</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -864,13 +1730,13 @@
         <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5">
         <v>60161679</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -884,13 +1750,13 @@
         <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>60161585</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -901,13 +1767,13 @@
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>60161708</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -918,13 +1784,13 @@
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E9">
         <v>60161882</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,13 +1804,13 @@
         <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E11">
         <v>60161739</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -955,13 +1821,13 @@
         <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E12">
         <v>60161749</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -972,13 +1838,13 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>60161885</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -992,13 +1858,13 @@
         <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15">
         <v>60161788</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1009,13 +1875,13 @@
         <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E16">
         <v>60161799</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1026,217 +1892,13 @@
         <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E17">
         <v>60161887</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666AD224-D931-1143-89FE-A13359F405FC}">
-  <dimension ref="A1:F37"/>
-  <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="31" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1334,7 +1996,7 @@
         <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Move into slurm_final folder
</commit_message>
<xml_diff>
--- a/conditions_files.xlsx
+++ b/conditions_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliabertoldo/My Drive (giuliabertoldo94@gmail.com)/work/github/thesis_ms_statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587A7093-B1A8-4B4D-9B06-DD5B834F0063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4EDCB9-835C-C140-AD3C-FA8BCBD62C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19040" xr2:uid="{1517BCBC-466E-C141-BBA8-2A6C10CC7C76}"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="214">
   <si>
     <t>test_pb_no_orb_no_k_15.csv</t>
   </si>
@@ -662,6 +662,24 @@
   </si>
   <si>
     <t>55016271_*</t>
+  </si>
+  <si>
+    <t>55016686_*</t>
+  </si>
+  <si>
+    <t>pb_str_orb_no_k_70_slurm_job_78.slurm</t>
+  </si>
+  <si>
+    <t>sim_parallel_pb_str_orb_no_k_70_slurm_job_78.R</t>
+  </si>
+  <si>
+    <t>55016817_*</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* 40 minutes, interrupted and then I looked for the missing condition and just run that condition (see below)</t>
   </si>
 </sst>
 </file>
@@ -692,12 +710,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -712,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -720,7 +744,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,18 +1061,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666AD224-D931-1143-89FE-A13359F405FC}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="6"/>
   </cols>
@@ -1306,27 +1332,36 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>159</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" t="s">
+        <v>169</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="F17" s="6">
+      <c r="J17" s="8">
         <v>46</v>
       </c>
-      <c r="G17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>92</v>
       </c>
@@ -1349,7 +1384,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>33</v>
       </c>
@@ -1362,14 +1397,14 @@
       <c r="E20" t="s">
         <v>206</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>13</v>
       </c>
       <c r="G20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -1389,7 +1424,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>96</v>
       </c>
@@ -1412,7 +1447,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>52</v>
       </c>
@@ -1432,7 +1467,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1453,7 +1488,7 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>95</v>
       </c>
@@ -1476,7 +1511,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>40</v>
       </c>
@@ -1496,7 +1531,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>41</v>
       </c>
@@ -1516,7 +1551,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>97</v>
       </c>
@@ -1539,7 +1574,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>59</v>
       </c>
@@ -1640,6 +1675,20 @@
       </c>
       <c r="G37" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" t="s">
+        <v>211</v>
+      </c>
+      <c r="F39" s="6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>